<commit_message>
Last Commit - UiPath Performer
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\UiPath Demo-Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\UiPath Demo-Performer\UiPath-Demo-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74CFDA5-67AC-4FD4-B4E7-9EB3090E28AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB0C23E-2059-4471-B792-8A22B5E47D12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="48" windowWidth="17304" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>UiDemoExecutablePath</t>
   </si>
   <si>
-    <t>C:\Users\HP\Documents\UiPath</t>
-  </si>
-  <si>
     <t>UiDemoCredential</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>UiDemoQueue</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\UiPath\UIDemo.exe</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -553,10 +553,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -579,15 +579,15 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>